<commit_message>
Finished parts list for usb-uart schematic rev1.00
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Part Number</t>
   </si>
@@ -39,13 +39,108 @@
   </si>
   <si>
     <t xml:space="preserve">USB-UART </t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>08055C104JAT2A</t>
+  </si>
+  <si>
+    <t>08055A470JAT2A</t>
+  </si>
+  <si>
+    <t>47pF</t>
+  </si>
+  <si>
+    <t>ERJ-P06J472V</t>
+  </si>
+  <si>
+    <r>
+      <t>4.7k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>ERJ-P06J103V</t>
+  </si>
+  <si>
+    <r>
+      <t>10k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>10118194-0001LF</t>
+  </si>
+  <si>
+    <t>USB mini B</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ271V</t>
+  </si>
+  <si>
+    <r>
+      <t>270</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>5988170107F</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>ERJ-6GEY0R00V</t>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +155,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,9 +190,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -401,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +524,7 @@
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +534,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -436,8 +549,132 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/avx-corporation/08055C104JAT2A/478-3352-1-ND/930144","Digikey - 478-3352-1-ND")</f>
+        <v>Digikey - 478-3352-1-ND</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/avx-corporation/08055A470JAT2A/478-1312-1-ND/564344","Digikey - 478-1312-1-ND")</f>
+        <v>Digikey - 478-1312-1-ND</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-P06J472V/P4.7KADCT-ND/525517","Digikey -  P4.7KADCT-ND")</f>
+        <v>Digikey -  P4.7KADCT-ND</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-P06J103V/P10KADCT-ND/525438","Digikey - P10KADCT-ND")</f>
+        <v>Digikey - P10KADCT-ND</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/amphenol-fci/10118194-0001LF/609-4618-1-ND/2785382","Digikey - 609-4618-1-ND")</f>
+        <v>Digikey - 609-4618-1-ND</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-search/en?keywords=P270ACT-ND","Digikey - P270ACT-ND")</f>
+        <v>Digikey - P270ACT-ND</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/dialight/5988170107F/350-2044-1-ND/1291348","Digikey - 350-2044-1-ND")</f>
+        <v>Digikey - 350-2044-1-ND</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-6GEY0R00V/P0.0ACT-ND/82955","Digikey - P0.0ACT-ND")</f>
+        <v>Digikey - P0.0ACT-ND</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on uC schematic
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Part Number</t>
   </si>
@@ -134,6 +135,18 @@
       </rPr>
       <t>Ω</t>
     </r>
+  </si>
+  <si>
+    <t>LPC1768FBD100,551</t>
+  </si>
+  <si>
+    <t>uC</t>
+  </si>
+  <si>
+    <t>445C35A12M00000</t>
+  </si>
+  <si>
+    <t>12MHz crystal</t>
   </si>
 </sst>
 </file>
@@ -511,15 +524,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
   </cols>
@@ -565,7 +578,7 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -670,6 +683,36 @@
         <v>21</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>HYPERLINK("https://octopart.com/lpc1768fbd100%2C551-nxp+semiconductors-11854624","Octopart")</f>
+        <v>Octopart</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/cts-frequency-controls/445C35A12M00000/CTX1435CT-ND/5875920","Digikey - CTX1435CT-ND")</f>
+        <v>Digikey - CTX1435CT-ND</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
founda quad encoder and schmitt trigger inverter for debounce circuits
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Part Number</t>
   </si>
@@ -147,6 +147,36 @@
   </si>
   <si>
     <t>12MHz crystal</t>
+  </si>
+  <si>
+    <t>08055A180JAT2A</t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>FX135A-327</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
+  </si>
+  <si>
+    <t>08051A200JAT2A</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>EN11-HSM1BF20</t>
+  </si>
+  <si>
+    <t>Quad Encoder</t>
+  </si>
+  <si>
+    <t>74HC14D,653</t>
+  </si>
+  <si>
+    <t>6x Schmitt trigger inverter</t>
   </si>
 </sst>
 </file>
@@ -524,17 +554,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -683,7 +713,7 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -713,6 +743,81 @@
         <v>25</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/avx-corporation/08055A180JAT2A/478-1307-1-ND/564339","Digikey - 478-1307-1-ND")</f>
+        <v>Digikey - 478-1307-1-ND</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/fox-electronics/FX135A-327/631-1002-1-ND/1024707","Digikey - 631-1002-1-ND")</f>
+        <v>Digikey - 631-1002-1-ND</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/avx-corporation/08051A200JAT2A/478-3735-1-ND/1116433","Digikey - 478-3735-1-ND")</f>
+        <v>Digikey - 478-3735-1-ND</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/tt-electronics-bi/EN11-HSM1BF20/987-1398-ND/2620667","Digikey - 987-1398-ND")</f>
+        <v>Digikey - 987-1398-ND</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/nxp-semiconductors/74HC14D,653/568-1401-1-ND/763376","Digikey - 568-1401-1-ND")</f>
+        <v>Digikey - 568-1401-1-ND</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
         <v>1</v>
       </c>
     </row>

</xml_diff>